<commit_message>
Ajuste do cadastro de pessoas em massa, para enviar convite por e-mail.
</commit_message>
<xml_diff>
--- a/modelos/modelo_convite_pessoas_em_massa.xlsx
+++ b/modelos/modelo_convite_pessoas_em_massa.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t xml:space="preserve">nome_completo</t>
   </si>
@@ -37,25 +37,28 @@
     <t xml:space="preserve">projetos (códigos separados por vírgula) (opcional)</t>
   </si>
   <si>
-    <t xml:space="preserve">Sandra de Sá</t>
+    <t xml:space="preserve">Toni Garrido</t>
   </si>
   <si>
     <t xml:space="preserve">técnico</t>
   </si>
   <si>
-    <t xml:space="preserve">sandra@sa.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cod/10, cod/04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vinícius de Moraes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">financeiro</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vini@moraes.com</t>
+    <t xml:space="preserve">renato@ispn.org.br</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cod/04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Toni Beloto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jenipapos@yahoo.com.br</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paulo Miklos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">renato@renato.org.br</t>
   </si>
 </sst>
 </file>
@@ -168,13 +171,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.76"/>
@@ -210,6 +213,9 @@
       <c r="C2" s="0" t="s">
         <v>7</v>
       </c>
+      <c r="D2" s="0" t="n">
+        <v>666666</v>
+      </c>
       <c r="E2" s="0" t="s">
         <v>8</v>
       </c>
@@ -219,20 +225,33 @@
         <v>9</v>
       </c>
       <c r="B3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="D3" s="0" t="n">
+        <v>55555</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="0" t="n">
-        <v>546521</v>
-      </c>
-    </row>
+      <c r="B4" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="sandra@sa.com"/>
-    <hyperlink ref="C3" r:id="rId2" display="vini@moraes.com"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>